<commit_message>
Latest job posting and updated source file
</commit_message>
<xml_diff>
--- a/data/resume.xlsx
+++ b/data/resume.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\R\CV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daviddobrowski/Documents/R/CV/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58892129-3D56-4D42-B375-418F408B83BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9508D27E-4E2C-C246-A19C-A88B573823CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42240" yWindow="1905" windowWidth="29430" windowHeight="18375" activeTab="3" xr2:uid="{97808E7A-D4B8-4E3C-A894-F6504AE230E5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22260" activeTab="4" xr2:uid="{97808E7A-D4B8-4E3C-A894-F6504AE230E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="135">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -412,13 +412,37 @@
   </si>
   <si>
     <t>with honors in the liberal arts summa cum laude</t>
+  </si>
+  <si>
+    <t>Utilize R and SQL to collect, analyze, and report complex data sets and supervise others in the process </t>
+  </si>
+  <si>
+    <t>Perform sophisticated analytics and apply advanced strategies using visualizations to communicate data-informed insights to a diverse audience </t>
+  </si>
+  <si>
+    <t>Draw conclusions from multiple data sets to inform and guide collaborative action teams in an effort to identify strategic priorities and implement improvement plans </t>
+  </si>
+  <si>
+    <t>Identify and understand performance gaps and provide deep analysis of strengths and needs according to state and local indicators </t>
+  </si>
+  <si>
+    <t>Work collaboratively with school districts and local agencies in the process of identifying equity gaps and assist teams to align related actions and services</t>
+  </si>
+  <si>
+    <t>Direct research design projects using a wide variety of qualitative and quantitative research methods to determine the appropriate investment of resources to meet locally-defined goals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foster collaborative partnerships between and among educational, business and community groups and organizations for the purpose of advancing outcomes </t>
+  </si>
+  <si>
+    <t>Assist teams throughout the county by providing the technical data support and capacity building</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +462,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -460,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -473,6 +503,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,12 +824,12 @@
       <selection activeCell="A15" sqref="A15:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="13" width="23" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -818,12 +849,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -846,27 +877,27 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
@@ -874,22 +905,22 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
@@ -906,7 +937,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -924,9 +955,9 @@
       <selection activeCell="A19" sqref="A19:I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -964,7 +995,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1011,7 +1042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1031,12 +1062,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1059,27 +1090,27 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>44</v>
       </c>
@@ -1087,22 +1118,22 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1119,7 +1150,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1138,34 +1169,34 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1179,13 +1210,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{488CB500-FF21-E549-914F-7B77DBBD6FC3}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1205,7 +1236,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>62</v>
       </c>
@@ -1225,7 +1256,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>59</v>
       </c>
@@ -1253,17 +1284,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF11DD4-4A26-EC41-A750-30A6B386F243}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16" width="18.85546875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="16" width="18.83203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
@@ -1322,7 +1355,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -1335,8 +1368,32 @@
       <c r="D2" s="2">
         <v>43449</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="262.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="262.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -1386,7 +1443,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="262.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="262.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -1445,7 +1502,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>105</v>
       </c>
@@ -1468,7 +1525,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>105</v>
       </c>
@@ -1491,12 +1548,33 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B7"/>
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8"/>
+    </row>
+    <row r="18" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F24" s="6"/>
+    </row>
+    <row r="27" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F27" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1513,12 +1591,12 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="15" width="31.42578125" style="1" customWidth="1"/>
+    <col min="1" max="15" width="31.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1526,32 +1604,32 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1575,19 +1653,19 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="36" width="19.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="96.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="36" width="19.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>79</v>
       </c>
@@ -1598,7 +1676,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -1609,7 +1687,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>81</v>
       </c>
@@ -1620,7 +1698,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>82</v>
       </c>
@@ -1631,7 +1709,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>83</v>
       </c>
@@ -1642,7 +1720,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>84</v>
       </c>
@@ -1653,7 +1731,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>85</v>
       </c>
@@ -1664,7 +1742,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>86</v>
       </c>
@@ -1675,7 +1753,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
Fixed job decscriptions items
</commit_message>
<xml_diff>
--- a/data/resume.xlsx
+++ b/data/resume.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daviddobrowski/Documents/R/CV/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9508D27E-4E2C-C246-A19C-A88B573823CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639F4DDF-015D-034C-8DC9-2E83B7F2B758}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22260" activeTab="4" xr2:uid="{97808E7A-D4B8-4E3C-A894-F6504AE230E5}"/>
+    <workbookView xWindow="8900" yWindow="6500" windowWidth="23000" windowHeight="16100" activeTab="5" xr2:uid="{97808E7A-D4B8-4E3C-A894-F6504AE230E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="136">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -354,9 +354,6 @@
     <t xml:space="preserve">The Caledonian School </t>
   </si>
   <si>
-    <t xml:space="preserve">County of Santa Cruz Employee of Year Gold????  </t>
-  </si>
-  <si>
     <t>desc1</t>
   </si>
   <si>
@@ -436,6 +433,12 @@
   </si>
   <si>
     <t>Assist teams throughout the county by providing the technical data support and capacity building</t>
+  </si>
+  <si>
+    <t>County of Santa Cruz Employee of Year Gold</t>
+  </si>
+  <si>
+    <t>Clients</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1181,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
@@ -1233,7 +1236,7 @@
         <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -1250,10 +1253,10 @@
         <v>38487</v>
       </c>
       <c r="E2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" t="s">
         <v>123</v>
-      </c>
-      <c r="F2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -1270,10 +1273,10 @@
         <v>36678</v>
       </c>
       <c r="E3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" t="s">
         <v>125</v>
-      </c>
-      <c r="F3" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1286,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF11DD4-4A26-EC41-A750-30A6B386F243}">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -1313,46 +1316,46 @@
         <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="48" x14ac:dyDescent="0.2">
@@ -1369,28 +1372,28 @@
         <v>43449</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="262.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1585,60 +1588,55 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71599D1-9EB4-4672-82AF-0B687864A941}">
-  <dimension ref="A2:O15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="15" width="31.5" style="1" customWidth="1"/>
+    <col min="1" max="14" width="31.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>39</v>
-      </c>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16"/>
+      <c r="B16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added conference and honors sections
</commit_message>
<xml_diff>
--- a/data/resume.xlsx
+++ b/data/resume.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daviddobrowski/Documents/R/CV/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639F4DDF-015D-034C-8DC9-2E83B7F2B758}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813311F2-079C-BB42-A2E7-4D04F3C95D57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8900" yWindow="6500" windowWidth="23000" windowHeight="16100" activeTab="5" xr2:uid="{97808E7A-D4B8-4E3C-A894-F6504AE230E5}"/>
+    <workbookView xWindow="8900" yWindow="6500" windowWidth="23000" windowHeight="16100" activeTab="2" xr2:uid="{97808E7A-D4B8-4E3C-A894-F6504AE230E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="148">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -267,9 +267,6 @@
     <t>Bay Area Academy</t>
   </si>
   <si>
-    <t xml:space="preserve">       </t>
-  </si>
-  <si>
     <t xml:space="preserve">Who Leaves Service and Why? How Evaluation can help Programs Improve Service Retention. </t>
   </si>
   <si>
@@ -435,10 +432,49 @@
     <t>Assist teams throughout the county by providing the technical data support and capacity building</t>
   </si>
   <si>
-    <t>County of Santa Cruz Employee of Year Gold</t>
-  </si>
-  <si>
     <t>Clients</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>place</t>
+  </si>
+  <si>
+    <t>Using ggplot and R: Demonstration of Visualization Principles in Practice</t>
+  </si>
+  <si>
+    <t>San Diego, CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  May 2021</t>
+  </si>
+  <si>
+    <t>honors</t>
+  </si>
+  <si>
+    <t>County of Santa Cruz</t>
+  </si>
+  <si>
+    <t>Community Foundation for Monterey County</t>
+  </si>
+  <si>
+    <t>Mid-Career Fellow</t>
+  </si>
+  <si>
+    <t>American Evaluation Association</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Merit Scholar  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Monterey Institute of International Studies</t>
+  </si>
+  <si>
+    <t>Ohio State University</t>
+  </si>
+  <si>
+    <t>Annual Employee of Recognition Award - Gold</t>
   </si>
 </sst>
 </file>
@@ -493,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -507,6 +543,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -955,7 +994,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:I19"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1166,42 +1205,78 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE8FAD3-42A0-445E-BC7D-E9DDDCA5417C}">
-  <dimension ref="A2:A7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
         <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -1236,7 +1311,7 @@
         <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -1253,10 +1328,10 @@
         <v>38487</v>
       </c>
       <c r="E2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" t="s">
         <v>122</v>
-      </c>
-      <c r="F2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -1273,10 +1348,10 @@
         <v>36678</v>
       </c>
       <c r="E3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" t="s">
         <v>124</v>
-      </c>
-      <c r="F3" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1316,46 +1391,46 @@
         <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="48" x14ac:dyDescent="0.2">
@@ -1372,28 +1447,28 @@
         <v>43449</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="262.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1507,13 +1582,13 @@
     </row>
     <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="2">
         <v>37135</v>
@@ -1530,13 +1605,13 @@
     </row>
     <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
         <v>102</v>
-      </c>
-      <c r="C6" t="s">
-        <v>103</v>
       </c>
       <c r="D6" s="4">
         <v>36739</v>
@@ -1590,8 +1665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71599D1-9EB4-4672-82AF-0B687864A941}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1601,7 +1676,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -1645,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8620C1-EBAF-4EE0-B87B-DFACACA9E270}">
-  <dimension ref="A2:AJ11"/>
+  <dimension ref="A1:AJ11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1658,108 +1733,125 @@
     <col min="3" max="36" width="19.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>78</v>
+        <v>136</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>